<commit_message>
Making sure my changes are comitted.
</commit_message>
<xml_diff>
--- a/Raw Data/DENU_2020_demography.xlsx
+++ b/Raw Data/DENU_2020_demography.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LTREB\LTREB_Phenology_Demography\Pheno_Demo\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840DEA9B-0D7B-484B-96AF-5F6A05FAD530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B92DF3-504B-47F9-B5EA-B7CB5478AFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="metadata" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1444,9 +1445,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1460,6 +1458,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1778,7 +1779,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A491" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E503" sqref="E503"/>
+      <selection pane="bottomLeft" activeCell="G504" sqref="G504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -45308,7 +45309,7 @@
       <c r="D551" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E551" s="45">
+      <c r="E551" s="44">
         <v>24</v>
       </c>
       <c r="F551" s="3" t="s">
@@ -45389,7 +45390,7 @@
       <c r="D552" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E552" s="45">
+      <c r="E552" s="44">
         <v>24</v>
       </c>
       <c r="F552" s="3" t="s">
@@ -45470,7 +45471,7 @@
       <c r="D553" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E553" s="45">
+      <c r="E553" s="44">
         <v>24</v>
       </c>
       <c r="F553" s="3" t="s">
@@ -45551,7 +45552,7 @@
       <c r="D554" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E554" s="45">
+      <c r="E554" s="44">
         <v>24</v>
       </c>
       <c r="F554" s="3" t="s">
@@ -81069,31 +81070,31 @@
       </c>
     </row>
     <row r="993" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A993" s="46">
-        <v>2020</v>
-      </c>
-      <c r="B993" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C993" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="D993" s="46" t="s">
+      <c r="A993" s="45">
+        <v>2020</v>
+      </c>
+      <c r="B993" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C993" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D993" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E993" s="47">
+      <c r="E993" s="46">
         <v>271</v>
       </c>
-      <c r="F993" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="G993" s="47" t="s">
+      <c r="F993" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G993" s="46" t="s">
         <v>367</v>
       </c>
-      <c r="H993" s="48">
+      <c r="H993" s="47">
         <v>956</v>
       </c>
-      <c r="I993" s="48">
+      <c r="I993" s="47">
         <v>3</v>
       </c>
       <c r="J993" s="1" t="s">
@@ -81816,7 +81817,7 @@
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="48" t="s">
         <v>369</v>
       </c>
     </row>
@@ -92633,10 +92634,10 @@
       <c r="F1" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="44"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
@@ -93375,6 +93376,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C27C2BB6D3449146994A382E4B983F24" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3916ea7ee4cb71b83dbe8cee805c736a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9ea4a38b-8811-4417-ad95-e83ecafd41d9" xmlns:ns4="8d30a389-4d56-4429-bc7f-f48221d5bec2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fd03811884ea603ed2e0d0d5adcc7f6" ns3:_="" ns4:_="">
     <xsd:import namespace="9ea4a38b-8811-4417-ad95-e83ecafd41d9"/>
@@ -93603,36 +93619,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC6D7EE0-C26E-46E6-9A2F-09BEADAE143D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B66E161F-3B67-47ED-8D2C-1E0620BA08C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9ea4a38b-8811-4417-ad95-e83ecafd41d9"/>
-    <ds:schemaRef ds:uri="8d30a389-4d56-4429-bc7f-f48221d5bec2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -93655,9 +93645,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B66E161F-3B67-47ED-8D2C-1E0620BA08C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC6D7EE0-C26E-46E6-9A2F-09BEADAE143D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9ea4a38b-8811-4417-ad95-e83ecafd41d9"/>
+    <ds:schemaRef ds:uri="8d30a389-4d56-4429-bc7f-f48221d5bec2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Making new phenology 2024 file 12.12.24 Merging two files that had the last DENU phenology survey data for 2024:
Also removing all the other sheets in the file (prior demography sheets and blank datasheet)

12.13.24
put a "1" in florivory for A.98.NA on 6/19 and A.201.GD  because note said hole in flower.

12.14.24
deleted "delete" column after consulting with Fatima who says it was notes to the data-takers about which plants to skip because they were done.
DENU.B.230.BS added uniqueID on 6/26 - cell was blank
Removing blank lines (no data taken for those plants on those days).  Up through 7/10 because I just figured out that blank lines that day aren't correct.
Fixes to 7/10 coming in separate commit.
</commit_message>
<xml_diff>
--- a/Raw Data/DENU_2020_demography.xlsx
+++ b/Raw Data/DENU_2020_demography.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LTREB\LTREB_Phenology_Demography\Pheno_Demo\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B92DF3-504B-47F9-B5EA-B7CB5478AFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1F98BC-3F5B-46F9-9DBE-BF298D21D565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demography" sheetId="3" r:id="rId1"/>
@@ -18,8 +18,7 @@
     <sheet name="phenology" sheetId="2" r:id="rId3"/>
     <sheet name="metadata" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17598" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17601" uniqueCount="375">
   <si>
     <t>Tag</t>
   </si>
@@ -1210,6 +1209,18 @@
   <si>
     <t>Added a row for B.271.NA which must have been tagged in 2019 but was first censused in 2022, where there is a note saying "not on datasheet"</t>
   </si>
+  <si>
+    <t>YSOD</t>
+  </si>
+  <si>
+    <t>12.16.24 Nora changed tag in datasheet from YS to YSOD, to be consistent with the same changes made by someone else in 2019, 2021 and continuing uses of YSOD after that</t>
+  </si>
+  <si>
+    <t>12.16.24</t>
+  </si>
+  <si>
+    <t>Nora changed tag in datasheet from YS to YSOD, to be consistent with the same changes made by someone else in 2019, 2021 and continuing uses of YSOD after that</t>
+  </si>
 </sst>
 </file>
 
@@ -1324,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1459,6 +1470,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1777,9 +1791,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A491" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G504" sqref="G504"/>
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z241" sqref="Z241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -20721,12 +20735,12 @@
       <c r="E241" s="16">
         <v>142</v>
       </c>
-      <c r="F241" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G241" s="16" t="str">
+      <c r="F241" s="50" t="s">
+        <v>371</v>
+      </c>
+      <c r="G241" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>DENU.A.142.YS</v>
+        <v>DENU.A.142.YSOD</v>
       </c>
       <c r="H241" s="38">
         <v>587</v>
@@ -20781,6 +20795,9 @@
       </c>
       <c r="Y241" s="3">
         <v>2</v>
+      </c>
+      <c r="Z241" s="45" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="242" spans="1:26" x14ac:dyDescent="0.35">
@@ -81808,10 +81825,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43002593-CCDD-4C00-A2C0-5FAE008DBA53}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -81824,6 +81841,16 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="48" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -93376,18 +93403,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -93620,14 +93647,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B66E161F-3B67-47ED-8D2C-1E0620BA08C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E4DFC38-782E-4182-9FF4-28D3F9BE294F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -93640,6 +93659,14 @@
     <ds:schemaRef ds:uri="8d30a389-4d56-4429-bc7f-f48221d5bec2"/>
     <ds:schemaRef ds:uri="9ea4a38b-8811-4417-ad95-e83ecafd41d9"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B66E161F-3B67-47ED-8D2C-1E0620BA08C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Changing phenology 2024 file name to match other years
</commit_message>
<xml_diff>
--- a/Raw Data/DENU_2020_demography.xlsx
+++ b/Raw Data/DENU_2020_demography.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LTREB\LTREB_Phenology_Demography\Pheno_Demo\Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1F98BC-3F5B-46F9-9DBE-BF298D21D565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8525CF87-2EAC-429B-B14E-FB0FE8BA44CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81828,7 +81828,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>